<commit_message>
Added libs directory for common JS files. Updated P4D iframe src.
</commit_message>
<xml_diff>
--- a/treas_island_missions.xlsx
+++ b/treas_island_missions.xlsx
@@ -30,7 +30,7 @@
     <author>Andy</author>
   </authors>
   <commentList>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Flight</t>
   </si>
@@ -257,10 +257,19 @@
     <t>P4Dtiles</t>
   </si>
   <si>
-    <t>http://data.andylyons.org/google_tiles/ti_2018-02-17_flt03/index.html</t>
-  </si>
-  <si>
-    <t>http://data.andylyons.org/google_tiles/ti_2018-02-17_flt01/index.html</t>
+    <t>https://data.andylyons.org/google_tiles/ti_2018-02-17_flt01/index.html</t>
+  </si>
+  <si>
+    <t>https://data.andylyons.org/google_tiles/ti_2018-02-17_flt03/index.html</t>
+  </si>
+  <si>
+    <t>MissionDescription</t>
+  </si>
+  <si>
+    <t>Treasure Island (urban area), nadir grid mapping mission with 80/70 overlap,  250 ft, 107 images, 17 acres.</t>
+  </si>
+  <si>
+    <t>Treasure Island (urban area), nadir grid mapping mission with 80/70 overlap,  250 ft, 83 images, 14 acres.</t>
   </si>
 </sst>
 </file>
@@ -329,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -362,6 +371,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -644,13 +656,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W3" sqref="W3"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,19 +670,21 @@
     <col min="1" max="1" width="17.21875" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="9" width="12.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="19" width="12.33203125" customWidth="1"/>
-    <col min="20" max="20" width="22.109375" customWidth="1"/>
-    <col min="21" max="21" width="33.6640625" customWidth="1"/>
-    <col min="22" max="22" width="40.44140625" customWidth="1"/>
-    <col min="23" max="23" width="22.109375" customWidth="1"/>
-    <col min="24" max="24" width="55.44140625" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.44140625" customWidth="1"/>
+    <col min="6" max="10" width="12.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="20" width="12.33203125" customWidth="1"/>
+    <col min="21" max="21" width="22.109375" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" customWidth="1"/>
+    <col min="23" max="23" width="40.44140625" customWidth="1"/>
+    <col min="24" max="24" width="22.109375" customWidth="1"/>
+    <col min="25" max="25" width="55.44140625" customWidth="1"/>
+    <col min="26" max="26" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -684,68 +698,71 @@
         <v>0</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Y1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -758,69 +775,72 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="5">
         <v>0.42569444444444443</v>
       </c>
-      <c r="F2" s="5">
+      <c r="G2" s="5">
         <v>0.42986111111111108</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>107</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>80</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>70</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>250</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>1.31</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>1012</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>742</v>
       </c>
-      <c r="P2" s="6">
-        <f>N2*O2/43560</f>
+      <c r="Q2" s="6">
+        <f>O2*P2/43560</f>
         <v>17.238383838383839</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -833,67 +853,67 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="F3" s="5">
         <v>0.43194444444444446</v>
       </c>
-      <c r="F3" s="5">
+      <c r="G3" s="5">
         <v>0.43333333333333335</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>48</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>80</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>70</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>250</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>1.31</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>255</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>738</v>
       </c>
-      <c r="P3" s="6">
-        <f>N3*O3/43560</f>
+      <c r="Q3" s="6">
+        <f>O3*P3/43560</f>
         <v>4.3202479338842972</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="W3" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="W3" s="3"/>
-      <c r="X3" t="s">
+      <c r="X3" s="3"/>
+      <c r="Y3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -906,71 +926,73 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="5">
         <v>0.46388888888888885</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>0.46666666666666662</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>83</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>80</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>70</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>300</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>1.58</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>710</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>847</v>
       </c>
-      <c r="P4" s="6">
-        <f>N4*O4/43560</f>
+      <c r="Q4" s="6">
+        <f>O4*P4/43560</f>
         <v>13.805555555555555</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="W4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="W4" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X4" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
-      <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -983,17 +1005,17 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="3"/>
+      <c r="T5" s="1"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
-      <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1006,17 +1028,17 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="3"/>
+      <c r="T6" s="1"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1029,17 +1051,17 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="3"/>
+      <c r="T7" s="1"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1052,17 +1074,17 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="3"/>
+      <c r="T8" s="1"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="E9" s="5"/>
       <c r="F9" s="5"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1075,17 +1097,17 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="3"/>
+      <c r="T9" s="1"/>
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="E10" s="5"/>
       <c r="F10" s="5"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1098,17 +1120,17 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="3"/>
+      <c r="T10" s="1"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1121,17 +1143,17 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
-      <c r="T11" s="3"/>
+      <c r="T11" s="1"/>
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
-      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1144,17 +1166,17 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
-      <c r="T12" s="3"/>
+      <c r="T12" s="1"/>
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1167,17 +1189,17 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
-      <c r="T13" s="3"/>
+      <c r="T13" s="1"/>
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
-      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1190,17 +1212,17 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="3"/>
+      <c r="T14" s="1"/>
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1213,17 +1235,17 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="3"/>
+      <c r="T15" s="1"/>
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="X15" s="3"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="1"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1236,17 +1258,17 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
-      <c r="T16" s="3"/>
+      <c r="T16" s="1"/>
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
-    </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X16" s="3"/>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
-      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="1"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1259,17 +1281,17 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="3"/>
+      <c r="T17" s="1"/>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X17" s="3"/>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
-      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1282,17 +1304,17 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
-      <c r="T18" s="3"/>
+      <c r="T18" s="1"/>
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X18" s="3"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
-      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1305,17 +1327,17 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
-      <c r="T19" s="3"/>
+      <c r="T19" s="1"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X19" s="3"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
-      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1328,17 +1350,17 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
-      <c r="T20" s="3"/>
+      <c r="T20" s="1"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="5"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1351,17 +1373,17 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
-      <c r="T21" s="3"/>
+      <c r="T21" s="1"/>
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1374,17 +1396,17 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="3"/>
+      <c r="T22" s="1"/>
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X22" s="3"/>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="5"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1397,17 +1419,17 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="3"/>
+      <c r="T23" s="1"/>
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X23" s="3"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
-      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="5"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1420,17 +1442,17 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="3"/>
+      <c r="T24" s="1"/>
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X24" s="3"/>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="5"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1443,17 +1465,17 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="3"/>
+      <c r="T25" s="1"/>
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="X25" s="3"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
-      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="5"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1466,15 +1488,16 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="3"/>
+      <c r="T26" s="1"/>
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W4" r:id="rId1"/>
-    <hyperlink ref="W2" r:id="rId2"/>
+    <hyperlink ref="X4" r:id="rId1"/>
+    <hyperlink ref="X2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId3"/>

</xml_diff>